<commit_message>
initial core BE + initial docsdocs
</commit_message>
<xml_diff>
--- a/Final Project/docs/planning/planning.xlsx
+++ b/Final Project/docs/planning/planning.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/congdinh/Library/Mobile Documents/com~apple~CloudDocs/works/mentor/classes/HN24_FRF_FJB_03/Mock/ims-ninja/docs/planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungp\movie\Final Project\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C7867-00B7-4045-8D5F-F9DEC8F40FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A6C99D-B843-4FD0-A6A3-24F5624819C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2860" windowWidth="28480" windowHeight="17000" xr2:uid="{C19F09B8-63BC-4CE7-BFBE-7F2585E3E38B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="1" xr2:uid="{C19F09B8-63BC-4CE7-BFBE-7F2585E3E38B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -124,13 +123,85 @@
   </si>
   <si>
     <t>PENDING</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Design Database</t>
+  </si>
+  <si>
+    <t>Design UI on Figma</t>
+  </si>
+  <si>
+    <t>Skeleton for BE</t>
+  </si>
+  <si>
+    <t>Skeleton for FE</t>
+  </si>
+  <si>
+    <t>HTML Code for UI</t>
+  </si>
+  <si>
+    <t>14/3/2025</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>On Progress</t>
+  </si>
+  <si>
+    <t>15/3/2025</t>
+  </si>
+  <si>
+    <t>16/3/2025</t>
+  </si>
+  <si>
+    <t>18/3/2025</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Develop Basic User Management &amp; Ticket Booking Functionality</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>UserManagement</t>
+  </si>
+  <si>
+    <t>Inital Ticket Booking</t>
+  </si>
+  <si>
+    <t>Build models, controllers, and services for user authentication handling.
+Create unit tests for the authentication module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop API for account registration and login. Create unit test for module Authentication.
+</t>
+  </si>
+  <si>
+    <t>Design initial APIs to retrieve the list of movies and showtimes.</t>
+  </si>
+  <si>
+    <t>16 -17/3/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Ticket Booking &amp; Ticket Selling – Employee Management
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +229,27 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -259,11 +355,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -305,6 +412,73 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,23 +816,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612C22F7-DEDF-4EDF-AEE8-648848F99654}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.35546875" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.35546875" customWidth="1"/>
+    <col min="8" max="8" width="15.640625" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:9" ht="15.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -687,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="64">
+    <row r="2" spans="1:9" ht="70.75">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -710,7 +884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48">
+    <row r="3" spans="1:9" ht="42.45">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="6" t="s">
@@ -729,7 +903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="64">
+    <row r="4" spans="1:9" ht="70.75">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="6" t="s">
@@ -759,7 +933,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="64">
+    <row r="6" spans="1:9" ht="56.6">
       <c r="A6" s="15">
         <v>1</v>
       </c>
@@ -782,7 +956,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48">
+    <row r="7" spans="1:9" ht="42.45">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="6" t="s">
@@ -822,4 +996,514 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462C93F8-120E-4632-ABB3-2BBE6FCADDF9}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.78515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.35546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.92578125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="20">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="24">
+        <v>45994</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="27">
+        <v>1</v>
+      </c>
+      <c r="B8" s="27">
+        <v>2</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="46.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="20">
+        <v>2</v>
+      </c>
+      <c r="B14" s="20">
+        <v>3</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="46.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="14.15" customHeight="1">
+      <c r="A20" s="27">
+        <v>3</v>
+      </c>
+      <c r="B20" s="27">
+        <v>4</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.15" customHeight="1">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="46.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>